<commit_message>
✅ [CHORE] : Edit Database Design Assignment
</commit_message>
<xml_diff>
--- a/4th/Database_Design.xlsx
+++ b/4th/Database_Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365inha-my.sharepoint.com/personal/lux1937_office_inha_ac_kr/Documents/SOPT/Seminar/Hyosik-Joo/4th/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60D080F4-109B-4253-A8F2-62C856174CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="8_{60D080F4-109B-4253-A8F2-62C856174CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C01202C-18F7-4A1D-8B05-DFEDE5C5BE2A}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{AECD554E-C23A-4B51-B0F2-B7E57064F823}"/>
   </bookViews>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>WE SOPT SERVER 4차 세미나 과제 - 데이터베이스 설계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -129,10 +128,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>article-comment table</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>so funny</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -149,10 +144,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>article_like table</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -161,11 +152,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>article-user table</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>article 개체와 user 개체 연결</t>
+    <t>user_id (author)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1:1 관계 / Primary Key : id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1: N 관계 / Primary Key : id, Foreign Key : user_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Foreign Key : user_id, article_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M : N 관계 / Primary Key : id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>like table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comment table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2nd comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Foreign Key : article_id, user_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -272,7 +295,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -282,32 +305,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -624,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68580CBC-93E2-4F66-92A1-7D7462F9E753}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.6"/>
@@ -638,8 +655,8 @@
     <col min="4" max="4" width="13.375" style="1" customWidth="1"/>
     <col min="5" max="6" width="9" style="1"/>
     <col min="7" max="7" width="14.3125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="37.8125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="28.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="36.4375" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -650,317 +667,373 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="F4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3">
+        <v>111111</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A7" s="3">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3">
+        <v>222222</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A8" s="3">
+        <v>3</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3">
+        <v>333333</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A9" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="F4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="8"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="E12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <v>3</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A15" s="3">
+        <v>2</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3">
+        <v>2</v>
+      </c>
+      <c r="G15" s="3">
+        <v>3</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A16" s="3">
+        <v>3</v>
+      </c>
+      <c r="B16" s="3">
+        <v>3</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3">
+        <v>3</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>2</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A17" s="3">
         <v>4</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A6" s="4">
-        <v>1</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="B17" s="3">
+        <v>3</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3">
+        <v>4</v>
+      </c>
+      <c r="F17" s="3">
+        <v>3</v>
+      </c>
+      <c r="G17" s="3">
+        <v>3</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A18" s="3">
         <v>5</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2</v>
+      </c>
+      <c r="E18" s="3">
+        <v>5</v>
+      </c>
+      <c r="F18" s="3">
+        <v>2</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A19" s="3">
         <v>6</v>
       </c>
-      <c r="D6" s="4">
-        <v>111111</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="8"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A7" s="4">
-        <v>2</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="4">
-        <v>222222</v>
-      </c>
-      <c r="F7" s="4">
-        <v>2</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="8"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A8" s="4">
-        <v>3</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="4">
-        <v>333333</v>
-      </c>
-      <c r="F8" s="4">
-        <v>3</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="E12" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="J12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A14" s="4">
-        <v>1</v>
-      </c>
-      <c r="B14" s="4">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4">
-        <v>3</v>
-      </c>
-      <c r="E14" s="4">
-        <v>1</v>
-      </c>
-      <c r="F14" s="4">
-        <v>2</v>
-      </c>
-      <c r="G14" s="4">
-        <v>1</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="2">
-        <v>1</v>
-      </c>
-      <c r="K14" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A15" s="4">
-        <v>2</v>
-      </c>
-      <c r="B15" s="4">
-        <v>2</v>
-      </c>
-      <c r="C15" s="4">
-        <v>2</v>
-      </c>
-      <c r="E15" s="4">
-        <v>2</v>
-      </c>
-      <c r="F15" s="4">
-        <v>2</v>
-      </c>
-      <c r="G15" s="4">
-        <v>3</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J15" s="2">
-        <v>2</v>
-      </c>
-      <c r="K15" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A16" s="4">
-        <v>3</v>
-      </c>
-      <c r="B16" s="4">
-        <v>3</v>
-      </c>
-      <c r="C16" s="4">
-        <v>1</v>
-      </c>
-      <c r="E16" s="4">
-        <v>3</v>
-      </c>
-      <c r="F16" s="4">
-        <v>1</v>
-      </c>
-      <c r="G16" s="4">
-        <v>2</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J16" s="2">
-        <v>3</v>
-      </c>
-      <c r="K16" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A17" s="6" t="s">
+      <c r="B19" s="3">
+        <v>2</v>
+      </c>
+      <c r="C19" s="3">
+        <v>3</v>
+      </c>
+      <c r="E19" s="3">
+        <v>6</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3">
+        <v>3</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A20" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="E20" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A21" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="E17" s="4">
-        <v>4</v>
-      </c>
-      <c r="F17" s="4">
-        <v>3</v>
-      </c>
-      <c r="G17" s="4">
-        <v>3</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J17" s="2">
-        <v>1</v>
-      </c>
-      <c r="K17" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="J18" s="2">
-        <v>3</v>
-      </c>
-      <c r="K18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="J19" s="2">
-        <v>2</v>
-      </c>
-      <c r="K19" s="2">
-        <v>3</v>
-      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="E21" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="11">
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="E21:H21"/>
     <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A17:C17"/>
     <mergeCell ref="E12:H12"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="J12:K12"/>
-    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="F4:I4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
✨ [FEAT] : 5th Seminar Finished
</commit_message>
<xml_diff>
--- a/4th/Database_Design.xlsx
+++ b/4th/Database_Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365inha-my.sharepoint.com/personal/lux1937_office_inha_ac_kr/Documents/SOPT/Seminar/Hyosik-Joo/4th/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60D080F4-109B-4253-A8F2-62C856174CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="8_{60D080F4-109B-4253-A8F2-62C856174CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C01202C-18F7-4A1D-8B05-DFEDE5C5BE2A}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{AECD554E-C23A-4B51-B0F2-B7E57064F823}"/>
   </bookViews>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>WE SOPT SERVER 4차 세미나 과제 - 데이터베이스 설계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -129,10 +128,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>article-comment table</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>so funny</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -149,10 +144,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>article_like table</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -161,11 +152,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>article-user table</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>article 개체와 user 개체 연결</t>
+    <t>user_id (author)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1:1 관계 / Primary Key : id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1: N 관계 / Primary Key : id, Foreign Key : user_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Foreign Key : user_id, article_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M : N 관계 / Primary Key : id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>like table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comment table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2nd comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Foreign Key : article_id, user_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -272,7 +295,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -282,32 +305,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -624,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68580CBC-93E2-4F66-92A1-7D7462F9E753}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.6"/>
@@ -638,8 +655,8 @@
     <col min="4" max="4" width="13.375" style="1" customWidth="1"/>
     <col min="5" max="6" width="9" style="1"/>
     <col min="7" max="7" width="14.3125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="37.8125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="28.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="36.4375" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -650,317 +667,373 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="F4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3">
+        <v>111111</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A7" s="3">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3">
+        <v>222222</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A8" s="3">
+        <v>3</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3">
+        <v>333333</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A9" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="F4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="8"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="E12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <v>3</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A15" s="3">
+        <v>2</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3">
+        <v>2</v>
+      </c>
+      <c r="G15" s="3">
+        <v>3</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A16" s="3">
+        <v>3</v>
+      </c>
+      <c r="B16" s="3">
+        <v>3</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3">
+        <v>3</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>2</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A17" s="3">
         <v>4</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A6" s="4">
-        <v>1</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="B17" s="3">
+        <v>3</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3">
+        <v>4</v>
+      </c>
+      <c r="F17" s="3">
+        <v>3</v>
+      </c>
+      <c r="G17" s="3">
+        <v>3</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A18" s="3">
         <v>5</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2</v>
+      </c>
+      <c r="E18" s="3">
+        <v>5</v>
+      </c>
+      <c r="F18" s="3">
+        <v>2</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A19" s="3">
         <v>6</v>
       </c>
-      <c r="D6" s="4">
-        <v>111111</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="8"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A7" s="4">
-        <v>2</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="4">
-        <v>222222</v>
-      </c>
-      <c r="F7" s="4">
-        <v>2</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="8"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A8" s="4">
-        <v>3</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="4">
-        <v>333333</v>
-      </c>
-      <c r="F8" s="4">
-        <v>3</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="E12" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="J12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A14" s="4">
-        <v>1</v>
-      </c>
-      <c r="B14" s="4">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4">
-        <v>3</v>
-      </c>
-      <c r="E14" s="4">
-        <v>1</v>
-      </c>
-      <c r="F14" s="4">
-        <v>2</v>
-      </c>
-      <c r="G14" s="4">
-        <v>1</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="2">
-        <v>1</v>
-      </c>
-      <c r="K14" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A15" s="4">
-        <v>2</v>
-      </c>
-      <c r="B15" s="4">
-        <v>2</v>
-      </c>
-      <c r="C15" s="4">
-        <v>2</v>
-      </c>
-      <c r="E15" s="4">
-        <v>2</v>
-      </c>
-      <c r="F15" s="4">
-        <v>2</v>
-      </c>
-      <c r="G15" s="4">
-        <v>3</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J15" s="2">
-        <v>2</v>
-      </c>
-      <c r="K15" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A16" s="4">
-        <v>3</v>
-      </c>
-      <c r="B16" s="4">
-        <v>3</v>
-      </c>
-      <c r="C16" s="4">
-        <v>1</v>
-      </c>
-      <c r="E16" s="4">
-        <v>3</v>
-      </c>
-      <c r="F16" s="4">
-        <v>1</v>
-      </c>
-      <c r="G16" s="4">
-        <v>2</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J16" s="2">
-        <v>3</v>
-      </c>
-      <c r="K16" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A17" s="6" t="s">
+      <c r="B19" s="3">
+        <v>2</v>
+      </c>
+      <c r="C19" s="3">
+        <v>3</v>
+      </c>
+      <c r="E19" s="3">
+        <v>6</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3">
+        <v>3</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A20" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="E20" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A21" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="E17" s="4">
-        <v>4</v>
-      </c>
-      <c r="F17" s="4">
-        <v>3</v>
-      </c>
-      <c r="G17" s="4">
-        <v>3</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J17" s="2">
-        <v>1</v>
-      </c>
-      <c r="K17" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="J18" s="2">
-        <v>3</v>
-      </c>
-      <c r="K18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="J19" s="2">
-        <v>2</v>
-      </c>
-      <c r="K19" s="2">
-        <v>3</v>
-      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="E21" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="11">
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="E21:H21"/>
     <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A17:C17"/>
     <mergeCell ref="E12:H12"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="J12:K12"/>
-    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="F4:I4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>